<commit_message>
fixed issue with new experience bars not show leveling notification
</commit_message>
<xml_diff>
--- a/Planning Report/application sprint planner sprint1 23.12.19.xlsx
+++ b/Planning Report/application sprint planner sprint1 23.12.19.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070A661F-E250-49F5-9743-AEA356466E96}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7BC850-0DD2-4227-8FFC-305821DC18D6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="420" windowWidth="22395" windowHeight="12030" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1545" yWindow="705" windowWidth="24345" windowHeight="14040" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="11" r:id="rId1"/>
@@ -1433,6 +1433,40 @@
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
   </cellStyles>
   <dxfs count="90">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -2904,40 +2938,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border>
         <left style="thin">
           <color theme="0" tint="-0.24994659260841701"/>
@@ -3259,10 +3259,10 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Milestone description" dataDxfId="77"/>
-    <tableColumn id="7" xr3:uid="{C2AA6DD8-DBD1-4E89-A1EF-3287225D3E74}" name="Required" dataDxfId="76"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category" dataDxfId="75"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Estimated Duration" dataDxfId="74"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Milestone description" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{C2AA6DD8-DBD1-4E89-A1EF-3287225D3E74}" name="Required" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Estimated Duration" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Start" dataCellStyle="Date"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="No. Days" dataCellStyle="Comma [0]"/>
@@ -3542,8 +3542,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BM119"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="B64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="Y73" sqref="Y73"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="B58" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17488,7 +17488,7 @@
         <v>17</v>
       </c>
       <c r="E72" s="34">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F72" s="31"/>
       <c r="G72" s="32"/>
@@ -26828,56 +26828,56 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:BM8 J116:BM117 J88:BM91 J97:BM97 J72:BM73 J103:BM103 J83:BM86 J75:BM76 J10:BM10 J22:BM58 J61:BM70 J94:BM95">
-    <cfRule type="expression" dxfId="73" priority="247">
+    <cfRule type="expression" dxfId="77" priority="247">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:AN4">
-    <cfRule type="expression" dxfId="72" priority="253">
+    <cfRule type="expression" dxfId="76" priority="253">
       <formula>J$5&lt;=EOMONTH($J$5,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:BM4">
-    <cfRule type="expression" dxfId="71" priority="249">
+    <cfRule type="expression" dxfId="75" priority="249">
       <formula>AND(K$5&lt;=EOMONTH($J$5,2),K$5&gt;EOMONTH($J$5,0),K$5&gt;EOMONTH($J$5,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:BM4">
-    <cfRule type="expression" dxfId="70" priority="248">
+    <cfRule type="expression" dxfId="74" priority="248">
       <formula>AND(J$5&lt;=EOMONTH($J$5,1),J$5&gt;EOMONTH($J$5,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:BM8 J10:BM10 J22:BM116">
-    <cfRule type="expression" dxfId="69" priority="270" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="270" stopIfTrue="1">
       <formula>AND($D8="Low risk",J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="289" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="289" stopIfTrue="1">
       <formula>AND($D8="High risk",J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="307" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="307" stopIfTrue="1">
       <formula>AND($D8="On track",J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="308" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="308" stopIfTrue="1">
       <formula>AND($D8="Med risk",J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="309" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="309" stopIfTrue="1">
       <formula>AND(LEN($D8)=0,J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J117:BM117">
-    <cfRule type="expression" dxfId="64" priority="317" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="317" stopIfTrue="1">
       <formula>AND(#REF!="Low risk",J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="318" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="318" stopIfTrue="1">
       <formula>AND(#REF!="High risk",J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="319" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="319" stopIfTrue="1">
       <formula>AND(#REF!="On track",J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="320" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="320" stopIfTrue="1">
       <formula>AND(#REF!="Med risk",J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="321" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="321" stopIfTrue="1">
       <formula>AND(LEN(#REF!)=0,J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26896,24 +26896,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:BM9">
-    <cfRule type="expression" dxfId="59" priority="238">
+    <cfRule type="expression" dxfId="63" priority="238">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:BM9">
-    <cfRule type="expression" dxfId="58" priority="240" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="240" stopIfTrue="1">
       <formula>AND($D9="Low risk",J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="241" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="241" stopIfTrue="1">
       <formula>AND($D9="High risk",J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="242" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="242" stopIfTrue="1">
       <formula>AND($D9="On track",J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="243" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="243" stopIfTrue="1">
       <formula>AND($D9="Med risk",J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="244" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="244" stopIfTrue="1">
       <formula>AND(LEN($D9)=0,J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26932,7 +26932,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J80:BM80 J77:BM78">
-    <cfRule type="expression" dxfId="53" priority="222">
+    <cfRule type="expression" dxfId="57" priority="222">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26951,7 +26951,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J82:GC82">
-    <cfRule type="expression" dxfId="52" priority="213">
+    <cfRule type="expression" dxfId="56" priority="213">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26970,7 +26970,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J81:BM81 J79:BM79">
-    <cfRule type="expression" dxfId="51" priority="206">
+    <cfRule type="expression" dxfId="55" priority="206">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26989,7 +26989,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J59:BM60">
-    <cfRule type="expression" dxfId="50" priority="198">
+    <cfRule type="expression" dxfId="54" priority="198">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27008,7 +27008,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J87:GC87">
-    <cfRule type="expression" dxfId="49" priority="189">
+    <cfRule type="expression" dxfId="53" priority="189">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27027,7 +27027,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J98:GC99 J101:GC103 J106:GC106 J113:GC115">
-    <cfRule type="expression" dxfId="48" priority="182">
+    <cfRule type="expression" dxfId="52" priority="182">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27046,7 +27046,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J100:GC100">
-    <cfRule type="expression" dxfId="47" priority="174">
+    <cfRule type="expression" dxfId="51" priority="174">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27065,7 +27065,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J96:GC96">
-    <cfRule type="expression" dxfId="46" priority="165">
+    <cfRule type="expression" dxfId="50" priority="165">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27084,7 +27084,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J71:GC71">
-    <cfRule type="expression" dxfId="45" priority="157">
+    <cfRule type="expression" dxfId="49" priority="157">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27103,7 +27103,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J93:BM93">
-    <cfRule type="expression" dxfId="44" priority="149">
+    <cfRule type="expression" dxfId="48" priority="149">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27122,7 +27122,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J104:GC105">
-    <cfRule type="expression" dxfId="43" priority="141">
+    <cfRule type="expression" dxfId="47" priority="141">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27141,7 +27141,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J107:GC108">
-    <cfRule type="expression" dxfId="42" priority="133">
+    <cfRule type="expression" dxfId="46" priority="133">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27160,7 +27160,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J111:GC111">
-    <cfRule type="expression" dxfId="41" priority="125">
+    <cfRule type="expression" dxfId="45" priority="125">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27179,7 +27179,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J112:GC112">
-    <cfRule type="expression" dxfId="40" priority="117">
+    <cfRule type="expression" dxfId="44" priority="117">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27198,7 +27198,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J74:BM74">
-    <cfRule type="expression" dxfId="39" priority="101">
+    <cfRule type="expression" dxfId="43" priority="101">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27217,7 +27217,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J110:BM110">
-    <cfRule type="expression" dxfId="38" priority="93">
+    <cfRule type="expression" dxfId="42" priority="93">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27236,7 +27236,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J92:BM92">
-    <cfRule type="expression" dxfId="37" priority="61">
+    <cfRule type="expression" dxfId="41" priority="61">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27255,7 +27255,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J109:GC109">
-    <cfRule type="expression" dxfId="36" priority="69">
+    <cfRule type="expression" dxfId="40" priority="69">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27274,24 +27274,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:BM11">
-    <cfRule type="expression" dxfId="35" priority="45">
+    <cfRule type="expression" dxfId="39" priority="45">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:BM11">
-    <cfRule type="expression" dxfId="34" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="47" stopIfTrue="1">
       <formula>AND($D11="Low risk",J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="48" stopIfTrue="1">
       <formula>AND($D11="High risk",J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="49" stopIfTrue="1">
       <formula>AND($D11="On track",J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="50" stopIfTrue="1">
       <formula>AND($D11="Med risk",J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="51" stopIfTrue="1">
       <formula>AND(LEN($D11)=0,J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27310,24 +27310,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:BM14">
-    <cfRule type="expression" dxfId="29" priority="37">
+    <cfRule type="expression" dxfId="33" priority="37">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:BM14">
-    <cfRule type="expression" dxfId="28" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="39" stopIfTrue="1">
       <formula>AND($D12="Low risk",J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="40" stopIfTrue="1">
       <formula>AND($D12="High risk",J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="41" stopIfTrue="1">
       <formula>AND($D12="On track",J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="42" stopIfTrue="1">
       <formula>AND($D12="Med risk",J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="43" stopIfTrue="1">
       <formula>AND(LEN($D12)=0,J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27346,24 +27346,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:BM15">
-    <cfRule type="expression" dxfId="23" priority="29">
+    <cfRule type="expression" dxfId="27" priority="29">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:BM15">
-    <cfRule type="expression" dxfId="22" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="31" stopIfTrue="1">
       <formula>AND($D15="Low risk",J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="32" stopIfTrue="1">
       <formula>AND($D15="High risk",J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="33" stopIfTrue="1">
       <formula>AND($D15="On track",J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="34" stopIfTrue="1">
       <formula>AND($D15="Med risk",J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="35" stopIfTrue="1">
       <formula>AND(LEN($D15)=0,J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27382,46 +27382,46 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:BM18">
-    <cfRule type="expression" dxfId="17" priority="21">
+    <cfRule type="expression" dxfId="21" priority="21">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:BM18">
-    <cfRule type="expression" dxfId="16" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="23" stopIfTrue="1">
       <formula>AND($D16="Low risk",J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="24" stopIfTrue="1">
       <formula>AND($D16="High risk",J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="25" stopIfTrue="1">
       <formula>AND($D16="On track",J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="26" stopIfTrue="1">
       <formula>AND($D16="Med risk",J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="27" stopIfTrue="1">
       <formula>AND(LEN($D16)=0,J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19:BM19">
-    <cfRule type="expression" dxfId="11" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="16" stopIfTrue="1">
       <formula>AND($D19="Low risk",J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="17" stopIfTrue="1">
       <formula>AND($D19="High risk",J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="18" stopIfTrue="1">
       <formula>AND($D19="On track",J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="19" stopIfTrue="1">
       <formula>AND($D19="Med risk",J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="20" stopIfTrue="1">
       <formula>AND(LEN($D19)=0,J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19:BM19">
-    <cfRule type="expression" dxfId="6" priority="13">
+    <cfRule type="expression" dxfId="10" priority="13">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27440,19 +27440,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:BM21">
-    <cfRule type="expression" dxfId="5" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="8" stopIfTrue="1">
       <formula>AND($D20="Low risk",J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
       <formula>AND($D20="High risk",J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="10" stopIfTrue="1">
       <formula>AND($D20="On track",J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="11" stopIfTrue="1">
       <formula>AND($D20="Med risk",J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="12" stopIfTrue="1">
       <formula>AND(LEN($D20)=0,J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27471,7 +27471,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:GC21">
-    <cfRule type="expression" dxfId="0" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>